<commit_message>
Completed Minor Changes Without Quotations
</commit_message>
<xml_diff>
--- a/YandS.UI/Template/INVOICE_REP_TEMPLATE.xlsx
+++ b/YandS.UI/Template/INVOICE_REP_TEMPLATE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Working\yands\LegalSystem\YandS\YandS.UI\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Working\Git\i.am.cloud.developer@outlook.com\YandSLmS\YandS.UI\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9303D667-F0B6-4E4F-90D5-A89BCB2C3130}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E16F3CB-2AAA-403A-A506-DB1FDB49A92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -230,23 +230,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>169333</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>169334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331825</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>169334</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A2AB004-6069-4E71-880D-638956497A71}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA9551CA-291C-4047-A63D-9AEF745AF73D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -254,15 +254,22 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="11554" t="17508" r="11554" b="13219"/>
-        <a:stretch/>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="314325" y="238125"/>
-          <a:ext cx="1838325" cy="866775"/>
+          <a:off x="2338916" y="169334"/>
+          <a:ext cx="1464242" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -574,7 +581,7 @@
   <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>